<commit_message>
state capacity index based on 8 proxies and 3 categories
</commit_message>
<xml_diff>
--- a/data/interim/P5_composite_indicators.xlsx
+++ b/data/interim/P5_composite_indicators.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G420"/>
+  <dimension ref="A1:G433"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8080,332 +8080,332 @@
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>1991</v>
+        <v>2006</v>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D309" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E309" t="n">
         <v>0</v>
       </c>
       <c r="F309" t="n">
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="G309" t="n">
-        <v>-2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>1992</v>
+        <v>2007</v>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C310" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D310" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E310" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F310" t="n">
-        <v>-6</v>
+        <v>8</v>
       </c>
       <c r="G310" t="n">
-        <v>-6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>1993</v>
+        <v>2008</v>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C311" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D311" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E311" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F311" t="n">
-        <v>-6</v>
+        <v>8</v>
       </c>
       <c r="G311" t="n">
-        <v>-6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>1994</v>
+        <v>2009</v>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C312" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D312" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E312" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F312" t="n">
-        <v>-6</v>
+        <v>8</v>
       </c>
       <c r="G312" t="n">
-        <v>-6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>1995</v>
+        <v>2010</v>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C313" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D313" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E313" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F313" t="n">
-        <v>-6</v>
+        <v>8</v>
       </c>
       <c r="G313" t="n">
-        <v>-6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>1996</v>
+        <v>2011</v>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C314" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D314" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E314" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F314" t="n">
-        <v>-6</v>
+        <v>8</v>
       </c>
       <c r="G314" t="n">
-        <v>-6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>1997</v>
+        <v>2012</v>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C315" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D315" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E315" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F315" t="n">
-        <v>-5</v>
+        <v>8</v>
       </c>
       <c r="G315" t="n">
-        <v>-5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>1998</v>
+        <v>2013</v>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C316" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D316" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E316" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F316" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="G316" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>1999</v>
+        <v>2014</v>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C317" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D317" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E317" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F317" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="G317" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C318" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D318" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E318" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F318" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="G318" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>2001</v>
+        <v>2016</v>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C319" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D319" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E319" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F319" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="G319" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>2002</v>
+        <v>2017</v>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C320" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D320" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E320" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F320" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="G320" t="n">
-        <v>-1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>2003</v>
+        <v>2018</v>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="C321" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D321" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E321" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F321" t="n">
-        <v>-3</v>
+        <v>8</v>
       </c>
       <c r="G321" t="n">
-        <v>-3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>2004</v>
+        <v>1991</v>
       </c>
       <c r="B322" t="inlineStr">
         <is>
@@ -8416,21 +8416,21 @@
         <v>1</v>
       </c>
       <c r="D322" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E322" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F322" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="G322" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
-        <v>2005</v>
+        <v>1992</v>
       </c>
       <c r="B323" t="inlineStr">
         <is>
@@ -8438,24 +8438,24 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D323" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E323" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F323" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="G323" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>2006</v>
+        <v>1993</v>
       </c>
       <c r="B324" t="inlineStr">
         <is>
@@ -8463,24 +8463,24 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D324" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E324" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F324" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="G324" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>2007</v>
+        <v>1994</v>
       </c>
       <c r="B325" t="inlineStr">
         <is>
@@ -8488,24 +8488,24 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D325" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E325" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F325" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="G325" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>2008</v>
+        <v>1995</v>
       </c>
       <c r="B326" t="inlineStr">
         <is>
@@ -8513,24 +8513,24 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D326" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E326" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F326" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="G326" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>2009</v>
+        <v>1996</v>
       </c>
       <c r="B327" t="inlineStr">
         <is>
@@ -8538,24 +8538,24 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D327" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E327" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F327" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="G327" t="n">
-        <v>-3</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>2010</v>
+        <v>1997</v>
       </c>
       <c r="B328" t="inlineStr">
         <is>
@@ -8563,24 +8563,24 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D328" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E328" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F328" t="n">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="G328" t="n">
-        <v>-3</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>2011</v>
+        <v>1998</v>
       </c>
       <c r="B329" t="inlineStr">
         <is>
@@ -8588,24 +8588,24 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D329" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E329" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F329" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="G329" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>2012</v>
+        <v>1999</v>
       </c>
       <c r="B330" t="inlineStr">
         <is>
@@ -8613,24 +8613,24 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D330" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E330" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F330" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="G330" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>2013</v>
+        <v>2000</v>
       </c>
       <c r="B331" t="inlineStr">
         <is>
@@ -8638,24 +8638,24 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D331" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E331" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F331" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="G331" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>2014</v>
+        <v>2001</v>
       </c>
       <c r="B332" t="inlineStr">
         <is>
@@ -8663,24 +8663,24 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D332" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E332" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F332" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="G332" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>2015</v>
+        <v>2002</v>
       </c>
       <c r="B333" t="inlineStr">
         <is>
@@ -8688,24 +8688,24 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D333" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E333" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F333" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="G333" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>2016</v>
+        <v>2003</v>
       </c>
       <c r="B334" t="inlineStr">
         <is>
@@ -8719,7 +8719,7 @@
         <v>4</v>
       </c>
       <c r="E334" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F334" t="n">
         <v>-3</v>
@@ -8730,7 +8730,7 @@
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>2017</v>
+        <v>2004</v>
       </c>
       <c r="B335" t="inlineStr">
         <is>
@@ -8744,7 +8744,7 @@
         <v>4</v>
       </c>
       <c r="E335" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F335" t="n">
         <v>-3</v>
@@ -8755,7 +8755,7 @@
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="B336" t="inlineStr">
         <is>
@@ -8769,7 +8769,7 @@
         <v>4</v>
       </c>
       <c r="E336" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F336" t="n">
         <v>-3</v>
@@ -8780,332 +8780,332 @@
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>1991</v>
+        <v>2006</v>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C337" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D337" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E337" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F337" t="n">
-        <v>-8</v>
+        <v>-3</v>
       </c>
       <c r="G337" t="n">
-        <v>-8</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
-        <v>1992</v>
+        <v>2007</v>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C338" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D338" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E338" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F338" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G338" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>1993</v>
+        <v>2008</v>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C339" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D339" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E339" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F339" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G339" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>1994</v>
+        <v>2009</v>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C340" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D340" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E340" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F340" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G340" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
-        <v>1995</v>
+        <v>2010</v>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C341" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D341" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E341" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F341" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G341" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
-        <v>1996</v>
+        <v>2011</v>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C342" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D342" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E342" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F342" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G342" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>1997</v>
+        <v>2012</v>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C343" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D343" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E343" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F343" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G343" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>1998</v>
+        <v>2013</v>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C344" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D344" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E344" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F344" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G344" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>1999</v>
+        <v>2014</v>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C345" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D345" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E345" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F345" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G345" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="n">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C346" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D346" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E346" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F346" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G346" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>2001</v>
+        <v>2016</v>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C347" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D347" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E347" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F347" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G347" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>2002</v>
+        <v>2017</v>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C348" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D348" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E348" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F348" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G348" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>2003</v>
+        <v>2018</v>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C349" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D349" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E349" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F349" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="G349" t="n">
-        <v>-9</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>2004</v>
+        <v>1991</v>
       </c>
       <c r="B350" t="inlineStr">
         <is>
@@ -9116,21 +9116,21 @@
         <v>0</v>
       </c>
       <c r="D350" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E350" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F350" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="G350" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
-        <v>2005</v>
+        <v>1992</v>
       </c>
       <c r="B351" t="inlineStr">
         <is>
@@ -9144,7 +9144,7 @@
         <v>9</v>
       </c>
       <c r="E351" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F351" t="n">
         <v>-9</v>
@@ -9155,7 +9155,7 @@
     </row>
     <row r="352">
       <c r="A352" t="n">
-        <v>2006</v>
+        <v>1993</v>
       </c>
       <c r="B352" t="inlineStr">
         <is>
@@ -9169,7 +9169,7 @@
         <v>9</v>
       </c>
       <c r="E352" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F352" t="n">
         <v>-9</v>
@@ -9180,7 +9180,7 @@
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>2007</v>
+        <v>1994</v>
       </c>
       <c r="B353" t="inlineStr">
         <is>
@@ -9194,7 +9194,7 @@
         <v>9</v>
       </c>
       <c r="E353" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F353" t="n">
         <v>-9</v>
@@ -9205,7 +9205,7 @@
     </row>
     <row r="354">
       <c r="A354" t="n">
-        <v>2008</v>
+        <v>1995</v>
       </c>
       <c r="B354" t="inlineStr">
         <is>
@@ -9219,7 +9219,7 @@
         <v>9</v>
       </c>
       <c r="E354" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F354" t="n">
         <v>-9</v>
@@ -9230,7 +9230,7 @@
     </row>
     <row r="355">
       <c r="A355" t="n">
-        <v>2009</v>
+        <v>1996</v>
       </c>
       <c r="B355" t="inlineStr">
         <is>
@@ -9244,7 +9244,7 @@
         <v>9</v>
       </c>
       <c r="E355" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F355" t="n">
         <v>-9</v>
@@ -9255,7 +9255,7 @@
     </row>
     <row r="356">
       <c r="A356" t="n">
-        <v>2010</v>
+        <v>1997</v>
       </c>
       <c r="B356" t="inlineStr">
         <is>
@@ -9269,7 +9269,7 @@
         <v>9</v>
       </c>
       <c r="E356" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F356" t="n">
         <v>-9</v>
@@ -9280,7 +9280,7 @@
     </row>
     <row r="357">
       <c r="A357" t="n">
-        <v>2011</v>
+        <v>1998</v>
       </c>
       <c r="B357" t="inlineStr">
         <is>
@@ -9294,7 +9294,7 @@
         <v>9</v>
       </c>
       <c r="E357" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F357" t="n">
         <v>-9</v>
@@ -9305,7 +9305,7 @@
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>2012</v>
+        <v>1999</v>
       </c>
       <c r="B358" t="inlineStr">
         <is>
@@ -9319,7 +9319,7 @@
         <v>9</v>
       </c>
       <c r="E358" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F358" t="n">
         <v>-9</v>
@@ -9330,7 +9330,7 @@
     </row>
     <row r="359">
       <c r="A359" t="n">
-        <v>2013</v>
+        <v>2000</v>
       </c>
       <c r="B359" t="inlineStr">
         <is>
@@ -9341,21 +9341,21 @@
         <v>0</v>
       </c>
       <c r="D359" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E359" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F359" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="G359" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="n">
-        <v>2014</v>
+        <v>2001</v>
       </c>
       <c r="B360" t="inlineStr">
         <is>
@@ -9366,21 +9366,21 @@
         <v>0</v>
       </c>
       <c r="D360" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E360" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F360" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="G360" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="n">
-        <v>2015</v>
+        <v>2002</v>
       </c>
       <c r="B361" t="inlineStr">
         <is>
@@ -9391,21 +9391,21 @@
         <v>0</v>
       </c>
       <c r="D361" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E361" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F361" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="G361" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="n">
-        <v>2016</v>
+        <v>2003</v>
       </c>
       <c r="B362" t="inlineStr">
         <is>
@@ -9416,21 +9416,21 @@
         <v>0</v>
       </c>
       <c r="D362" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E362" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F362" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="G362" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="n">
-        <v>2017</v>
+        <v>2004</v>
       </c>
       <c r="B363" t="inlineStr">
         <is>
@@ -9441,21 +9441,21 @@
         <v>0</v>
       </c>
       <c r="D363" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E363" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F363" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="G363" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="B364" t="inlineStr">
         <is>
@@ -9466,346 +9466,346 @@
         <v>0</v>
       </c>
       <c r="D364" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E364" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F364" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="G364" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
-        <v>1991</v>
+        <v>2006</v>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C365" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D365" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E365" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F365" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
       <c r="G365" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
-        <v>1992</v>
+        <v>2007</v>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C366" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D366" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E366" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F366" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
       <c r="G366" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
-        <v>1993</v>
+        <v>2008</v>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C367" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D367" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E367" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F367" t="n">
-        <v>5</v>
+        <v>-9</v>
       </c>
       <c r="G367" t="n">
-        <v>5</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
-        <v>1994</v>
+        <v>2009</v>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C368" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D368" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E368" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F368" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
       <c r="G368" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="n">
-        <v>1995</v>
+        <v>2010</v>
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C369" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D369" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E369" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F369" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
       <c r="G369" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="n">
-        <v>1996</v>
+        <v>2011</v>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C370" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D370" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E370" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F370" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
       <c r="G370" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
-        <v>1997</v>
+        <v>2012</v>
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C371" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D371" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E371" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F371" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
       <c r="G371" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="n">
-        <v>1998</v>
+        <v>2013</v>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C372" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D372" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E372" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F372" t="n">
-        <v>7</v>
+        <v>-8</v>
       </c>
       <c r="G372" t="n">
-        <v>7</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="n">
-        <v>1999</v>
+        <v>2014</v>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C373" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D373" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E373" t="n">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F373" t="n">
-        <v>7</v>
+        <v>-8</v>
       </c>
       <c r="G373" t="n">
-        <v>7</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C374" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D374" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E374" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F374" t="n">
-        <v>6</v>
+        <v>-8</v>
       </c>
       <c r="G374" t="n">
-        <v>6</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
-        <v>2001</v>
+        <v>2016</v>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C375" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D375" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E375" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F375" t="n">
-        <v>6</v>
+        <v>-8</v>
       </c>
       <c r="G375" t="n">
-        <v>6</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
-        <v>2002</v>
+        <v>2017</v>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C376" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D376" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E376" t="n">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F376" t="n">
-        <v>6</v>
+        <v>-8</v>
       </c>
       <c r="G376" t="n">
-        <v>6</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="n">
-        <v>2003</v>
+        <v>2018</v>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C377" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D377" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E377" t="n">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F377" t="n">
-        <v>6</v>
+        <v>-8</v>
       </c>
       <c r="G377" t="n">
-        <v>6</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="n">
-        <v>2004</v>
+        <v>1991</v>
       </c>
       <c r="B378" t="inlineStr">
         <is>
@@ -9819,7 +9819,7 @@
         <v>0</v>
       </c>
       <c r="E378" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F378" t="n">
         <v>6</v>
@@ -9830,7 +9830,7 @@
     </row>
     <row r="379">
       <c r="A379" t="n">
-        <v>2005</v>
+        <v>1992</v>
       </c>
       <c r="B379" t="inlineStr">
         <is>
@@ -9844,7 +9844,7 @@
         <v>0</v>
       </c>
       <c r="E379" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F379" t="n">
         <v>6</v>
@@ -9855,7 +9855,7 @@
     </row>
     <row r="380">
       <c r="A380" t="n">
-        <v>2006</v>
+        <v>1993</v>
       </c>
       <c r="B380" t="inlineStr">
         <is>
@@ -9863,24 +9863,24 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D380" t="n">
         <v>0</v>
       </c>
       <c r="E380" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F380" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G380" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
-        <v>2007</v>
+        <v>1994</v>
       </c>
       <c r="B381" t="inlineStr">
         <is>
@@ -9894,7 +9894,7 @@
         <v>0</v>
       </c>
       <c r="E381" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F381" t="n">
         <v>7</v>
@@ -9905,7 +9905,7 @@
     </row>
     <row r="382">
       <c r="A382" t="n">
-        <v>2008</v>
+        <v>1995</v>
       </c>
       <c r="B382" t="inlineStr">
         <is>
@@ -9919,7 +9919,7 @@
         <v>0</v>
       </c>
       <c r="E382" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F382" t="n">
         <v>7</v>
@@ -9930,7 +9930,7 @@
     </row>
     <row r="383">
       <c r="A383" t="n">
-        <v>2009</v>
+        <v>1996</v>
       </c>
       <c r="B383" t="inlineStr">
         <is>
@@ -9944,7 +9944,7 @@
         <v>0</v>
       </c>
       <c r="E383" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F383" t="n">
         <v>7</v>
@@ -9955,7 +9955,7 @@
     </row>
     <row r="384">
       <c r="A384" t="n">
-        <v>2010</v>
+        <v>1997</v>
       </c>
       <c r="B384" t="inlineStr">
         <is>
@@ -9963,24 +9963,24 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D384" t="n">
         <v>0</v>
       </c>
       <c r="E384" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F384" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G384" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="n">
-        <v>2011</v>
+        <v>1998</v>
       </c>
       <c r="B385" t="inlineStr">
         <is>
@@ -9988,24 +9988,24 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D385" t="n">
         <v>0</v>
       </c>
       <c r="E385" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F385" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G385" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="n">
-        <v>2012</v>
+        <v>1999</v>
       </c>
       <c r="B386" t="inlineStr">
         <is>
@@ -10013,24 +10013,24 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D386" t="n">
         <v>0</v>
       </c>
       <c r="E386" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F386" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G386" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
-        <v>2013</v>
+        <v>2000</v>
       </c>
       <c r="B387" t="inlineStr">
         <is>
@@ -10044,7 +10044,7 @@
         <v>0</v>
       </c>
       <c r="E387" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F387" t="n">
         <v>6</v>
@@ -10055,7 +10055,7 @@
     </row>
     <row r="388">
       <c r="A388" t="n">
-        <v>2014</v>
+        <v>2001</v>
       </c>
       <c r="B388" t="inlineStr">
         <is>
@@ -10063,24 +10063,24 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D388" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E388" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F388" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G388" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="n">
-        <v>2015</v>
+        <v>2002</v>
       </c>
       <c r="B389" t="inlineStr">
         <is>
@@ -10088,24 +10088,24 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D389" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E389" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F389" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G389" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>2016</v>
+        <v>2003</v>
       </c>
       <c r="B390" t="inlineStr">
         <is>
@@ -10113,24 +10113,24 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D390" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E390" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F390" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G390" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
-        <v>2017</v>
+        <v>2004</v>
       </c>
       <c r="B391" t="inlineStr">
         <is>
@@ -10138,24 +10138,24 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D391" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E391" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F391" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G391" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="B392" t="inlineStr">
         <is>
@@ -10163,349 +10163,349 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D392" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E392" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F392" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G392" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
-        <v>1991</v>
+        <v>2006</v>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C393" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D393" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E393" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F393" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
       <c r="G393" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="n">
-        <v>1992</v>
+        <v>2007</v>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C394" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D394" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E394" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F394" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
       <c r="G394" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="n">
-        <v>1993</v>
+        <v>2008</v>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C395" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D395" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E395" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F395" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
       <c r="G395" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="n">
-        <v>1994</v>
+        <v>2009</v>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C396" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D396" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E396" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F396" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
       <c r="G396" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="n">
-        <v>1995</v>
+        <v>2010</v>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C397" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D397" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E397" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F397" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
       <c r="G397" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="n">
-        <v>1996</v>
+        <v>2011</v>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C398" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D398" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E398" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F398" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
       <c r="G398" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="n">
-        <v>1997</v>
+        <v>2012</v>
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C399" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D399" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E399" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F399" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
       <c r="G399" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="n">
-        <v>1998</v>
+        <v>2013</v>
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C400" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D400" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E400" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F400" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
       <c r="G400" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="n">
-        <v>1999</v>
+        <v>2014</v>
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C401" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D401" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E401" t="n">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F401" t="n">
-        <v>-9</v>
+        <v>4</v>
       </c>
       <c r="G401" t="n">
-        <v>-9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="n">
-        <v>2000</v>
+        <v>2015</v>
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C402" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D402" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E402" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F402" t="n">
-        <v>-9</v>
+        <v>4</v>
       </c>
       <c r="G402" t="n">
-        <v>-9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="n">
-        <v>2001</v>
+        <v>2016</v>
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C403" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D403" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E403" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F403" t="n">
-        <v>-9</v>
+        <v>4</v>
       </c>
       <c r="G403" t="n">
-        <v>-9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="n">
-        <v>2002</v>
+        <v>2017</v>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C404" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D404" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E404" t="n">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F404" t="n">
-        <v>-9</v>
+        <v>4</v>
       </c>
       <c r="G404" t="n">
-        <v>-9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="n">
-        <v>2003</v>
+        <v>2018</v>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C405" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D405" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E405" t="n">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F405" t="n">
-        <v>-9</v>
+        <v>4</v>
       </c>
       <c r="G405" t="n">
-        <v>-9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="n">
-        <v>2004</v>
+        <v>1991</v>
       </c>
       <c r="B406" t="inlineStr">
         <is>
@@ -10519,7 +10519,7 @@
         <v>9</v>
       </c>
       <c r="E406" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F406" t="n">
         <v>-9</v>
@@ -10530,7 +10530,7 @@
     </row>
     <row r="407">
       <c r="A407" t="n">
-        <v>2005</v>
+        <v>1992</v>
       </c>
       <c r="B407" t="inlineStr">
         <is>
@@ -10544,7 +10544,7 @@
         <v>9</v>
       </c>
       <c r="E407" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F407" t="n">
         <v>-9</v>
@@ -10555,7 +10555,7 @@
     </row>
     <row r="408">
       <c r="A408" t="n">
-        <v>2006</v>
+        <v>1993</v>
       </c>
       <c r="B408" t="inlineStr">
         <is>
@@ -10569,7 +10569,7 @@
         <v>9</v>
       </c>
       <c r="E408" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F408" t="n">
         <v>-9</v>
@@ -10580,7 +10580,7 @@
     </row>
     <row r="409">
       <c r="A409" t="n">
-        <v>2007</v>
+        <v>1994</v>
       </c>
       <c r="B409" t="inlineStr">
         <is>
@@ -10594,7 +10594,7 @@
         <v>9</v>
       </c>
       <c r="E409" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F409" t="n">
         <v>-9</v>
@@ -10605,7 +10605,7 @@
     </row>
     <row r="410">
       <c r="A410" t="n">
-        <v>2008</v>
+        <v>1995</v>
       </c>
       <c r="B410" t="inlineStr">
         <is>
@@ -10619,7 +10619,7 @@
         <v>9</v>
       </c>
       <c r="E410" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F410" t="n">
         <v>-9</v>
@@ -10630,7 +10630,7 @@
     </row>
     <row r="411">
       <c r="A411" t="n">
-        <v>2009</v>
+        <v>1996</v>
       </c>
       <c r="B411" t="inlineStr">
         <is>
@@ -10644,7 +10644,7 @@
         <v>9</v>
       </c>
       <c r="E411" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F411" t="n">
         <v>-9</v>
@@ -10655,7 +10655,7 @@
     </row>
     <row r="412">
       <c r="A412" t="n">
-        <v>2010</v>
+        <v>1997</v>
       </c>
       <c r="B412" t="inlineStr">
         <is>
@@ -10669,7 +10669,7 @@
         <v>9</v>
       </c>
       <c r="E412" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F412" t="n">
         <v>-9</v>
@@ -10680,7 +10680,7 @@
     </row>
     <row r="413">
       <c r="A413" t="n">
-        <v>2011</v>
+        <v>1998</v>
       </c>
       <c r="B413" t="inlineStr">
         <is>
@@ -10694,7 +10694,7 @@
         <v>9</v>
       </c>
       <c r="E413" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F413" t="n">
         <v>-9</v>
@@ -10705,7 +10705,7 @@
     </row>
     <row r="414">
       <c r="A414" t="n">
-        <v>2012</v>
+        <v>1999</v>
       </c>
       <c r="B414" t="inlineStr">
         <is>
@@ -10719,7 +10719,7 @@
         <v>9</v>
       </c>
       <c r="E414" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F414" t="n">
         <v>-9</v>
@@ -10730,7 +10730,7 @@
     </row>
     <row r="415">
       <c r="A415" t="n">
-        <v>2013</v>
+        <v>2000</v>
       </c>
       <c r="B415" t="inlineStr">
         <is>
@@ -10744,7 +10744,7 @@
         <v>9</v>
       </c>
       <c r="E415" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F415" t="n">
         <v>-9</v>
@@ -10755,7 +10755,7 @@
     </row>
     <row r="416">
       <c r="A416" t="n">
-        <v>2014</v>
+        <v>2001</v>
       </c>
       <c r="B416" t="inlineStr">
         <is>
@@ -10769,7 +10769,7 @@
         <v>9</v>
       </c>
       <c r="E416" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F416" t="n">
         <v>-9</v>
@@ -10780,7 +10780,7 @@
     </row>
     <row r="417">
       <c r="A417" t="n">
-        <v>2015</v>
+        <v>2002</v>
       </c>
       <c r="B417" t="inlineStr">
         <is>
@@ -10794,7 +10794,7 @@
         <v>9</v>
       </c>
       <c r="E417" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F417" t="n">
         <v>-9</v>
@@ -10805,7 +10805,7 @@
     </row>
     <row r="418">
       <c r="A418" t="n">
-        <v>2016</v>
+        <v>2003</v>
       </c>
       <c r="B418" t="inlineStr">
         <is>
@@ -10819,7 +10819,7 @@
         <v>9</v>
       </c>
       <c r="E418" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F418" t="n">
         <v>-9</v>
@@ -10830,7 +10830,7 @@
     </row>
     <row r="419">
       <c r="A419" t="n">
-        <v>2017</v>
+        <v>2004</v>
       </c>
       <c r="B419" t="inlineStr">
         <is>
@@ -10844,7 +10844,7 @@
         <v>9</v>
       </c>
       <c r="E419" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F419" t="n">
         <v>-9</v>
@@ -10855,7 +10855,7 @@
     </row>
     <row r="420">
       <c r="A420" t="n">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="B420" t="inlineStr">
         <is>
@@ -10869,12 +10869,337 @@
         <v>9</v>
       </c>
       <c r="E420" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F420" t="n">
         <v>-9</v>
       </c>
       <c r="G420" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="n">
+        <v>2006</v>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C421" t="n">
+        <v>0</v>
+      </c>
+      <c r="D421" t="n">
+        <v>9</v>
+      </c>
+      <c r="E421" t="n">
+        <v>15</v>
+      </c>
+      <c r="F421" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G421" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="n">
+        <v>2007</v>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C422" t="n">
+        <v>0</v>
+      </c>
+      <c r="D422" t="n">
+        <v>9</v>
+      </c>
+      <c r="E422" t="n">
+        <v>16</v>
+      </c>
+      <c r="F422" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G422" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="n">
+        <v>2008</v>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C423" t="n">
+        <v>0</v>
+      </c>
+      <c r="D423" t="n">
+        <v>9</v>
+      </c>
+      <c r="E423" t="n">
+        <v>17</v>
+      </c>
+      <c r="F423" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G423" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="n">
+        <v>2009</v>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C424" t="n">
+        <v>0</v>
+      </c>
+      <c r="D424" t="n">
+        <v>9</v>
+      </c>
+      <c r="E424" t="n">
+        <v>18</v>
+      </c>
+      <c r="F424" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G424" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C425" t="n">
+        <v>0</v>
+      </c>
+      <c r="D425" t="n">
+        <v>9</v>
+      </c>
+      <c r="E425" t="n">
+        <v>19</v>
+      </c>
+      <c r="F425" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G425" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C426" t="n">
+        <v>0</v>
+      </c>
+      <c r="D426" t="n">
+        <v>9</v>
+      </c>
+      <c r="E426" t="n">
+        <v>20</v>
+      </c>
+      <c r="F426" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G426" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C427" t="n">
+        <v>0</v>
+      </c>
+      <c r="D427" t="n">
+        <v>9</v>
+      </c>
+      <c r="E427" t="n">
+        <v>21</v>
+      </c>
+      <c r="F427" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G427" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C428" t="n">
+        <v>0</v>
+      </c>
+      <c r="D428" t="n">
+        <v>9</v>
+      </c>
+      <c r="E428" t="n">
+        <v>22</v>
+      </c>
+      <c r="F428" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G428" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C429" t="n">
+        <v>0</v>
+      </c>
+      <c r="D429" t="n">
+        <v>9</v>
+      </c>
+      <c r="E429" t="n">
+        <v>23</v>
+      </c>
+      <c r="F429" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G429" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C430" t="n">
+        <v>0</v>
+      </c>
+      <c r="D430" t="n">
+        <v>9</v>
+      </c>
+      <c r="E430" t="n">
+        <v>24</v>
+      </c>
+      <c r="F430" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G430" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C431" t="n">
+        <v>0</v>
+      </c>
+      <c r="D431" t="n">
+        <v>9</v>
+      </c>
+      <c r="E431" t="n">
+        <v>25</v>
+      </c>
+      <c r="F431" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G431" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C432" t="n">
+        <v>0</v>
+      </c>
+      <c r="D432" t="n">
+        <v>9</v>
+      </c>
+      <c r="E432" t="n">
+        <v>26</v>
+      </c>
+      <c r="F432" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G432" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>UZB</t>
+        </is>
+      </c>
+      <c r="C433" t="n">
+        <v>0</v>
+      </c>
+      <c r="D433" t="n">
+        <v>9</v>
+      </c>
+      <c r="E433" t="n">
+        <v>27</v>
+      </c>
+      <c r="F433" t="n">
+        <v>-9</v>
+      </c>
+      <c r="G433" t="n">
         <v>-9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
3 approaches _ template
</commit_message>
<xml_diff>
--- a/data/interim/P5_composite_indicators.xlsx
+++ b/data/interim/P5_composite_indicators.xlsx
@@ -8080,332 +8080,332 @@
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>2006</v>
+        <v>1991</v>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D309" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E309" t="n">
         <v>0</v>
       </c>
       <c r="F309" t="n">
-        <v>8</v>
+        <v>-2</v>
       </c>
       <c r="G309" t="n">
-        <v>8</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>2007</v>
+        <v>1992</v>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C310" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D310" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E310" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F310" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
       <c r="G310" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>2008</v>
+        <v>1993</v>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C311" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D311" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E311" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F311" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
       <c r="G311" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>2009</v>
+        <v>1994</v>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C312" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D312" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E312" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F312" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
       <c r="G312" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>2010</v>
+        <v>1995</v>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C313" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D313" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E313" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F313" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
       <c r="G313" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>2011</v>
+        <v>1996</v>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C314" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D314" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E314" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F314" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
       <c r="G314" t="n">
-        <v>8</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>2012</v>
+        <v>1997</v>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C315" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D315" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E315" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F315" t="n">
-        <v>8</v>
+        <v>-5</v>
       </c>
       <c r="G315" t="n">
-        <v>8</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>2013</v>
+        <v>1998</v>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C316" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D316" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E316" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F316" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="G316" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>2014</v>
+        <v>1999</v>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C317" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D317" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E317" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F317" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="G317" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C318" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D318" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E318" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F318" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="G318" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C319" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D319" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E319" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F319" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="G319" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>2017</v>
+        <v>2002</v>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C320" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D320" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E320" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F320" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="G320" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>2018</v>
+        <v>2003</v>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="C321" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D321" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E321" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F321" t="n">
-        <v>8</v>
+        <v>-3</v>
       </c>
       <c r="G321" t="n">
-        <v>8</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>1991</v>
+        <v>2004</v>
       </c>
       <c r="B322" t="inlineStr">
         <is>
@@ -8416,21 +8416,21 @@
         <v>1</v>
       </c>
       <c r="D322" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E322" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F322" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="G322" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
-        <v>1992</v>
+        <v>2005</v>
       </c>
       <c r="B323" t="inlineStr">
         <is>
@@ -8438,24 +8438,24 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D323" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E323" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F323" t="n">
-        <v>-6</v>
+        <v>-3</v>
       </c>
       <c r="G323" t="n">
-        <v>-6</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>1993</v>
+        <v>2006</v>
       </c>
       <c r="B324" t="inlineStr">
         <is>
@@ -8463,24 +8463,24 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D324" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E324" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F324" t="n">
-        <v>-6</v>
+        <v>-3</v>
       </c>
       <c r="G324" t="n">
-        <v>-6</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>1994</v>
+        <v>2007</v>
       </c>
       <c r="B325" t="inlineStr">
         <is>
@@ -8488,24 +8488,24 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D325" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E325" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F325" t="n">
-        <v>-6</v>
+        <v>-3</v>
       </c>
       <c r="G325" t="n">
-        <v>-6</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>1995</v>
+        <v>2008</v>
       </c>
       <c r="B326" t="inlineStr">
         <is>
@@ -8513,24 +8513,24 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D326" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E326" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F326" t="n">
-        <v>-6</v>
+        <v>-3</v>
       </c>
       <c r="G326" t="n">
-        <v>-6</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>1996</v>
+        <v>2009</v>
       </c>
       <c r="B327" t="inlineStr">
         <is>
@@ -8538,24 +8538,24 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D327" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E327" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F327" t="n">
-        <v>-6</v>
+        <v>-3</v>
       </c>
       <c r="G327" t="n">
-        <v>-6</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>1997</v>
+        <v>2010</v>
       </c>
       <c r="B328" t="inlineStr">
         <is>
@@ -8563,24 +8563,24 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D328" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E328" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F328" t="n">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="G328" t="n">
-        <v>-5</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>1998</v>
+        <v>2011</v>
       </c>
       <c r="B329" t="inlineStr">
         <is>
@@ -8588,24 +8588,24 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D329" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E329" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F329" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="G329" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>1999</v>
+        <v>2012</v>
       </c>
       <c r="B330" t="inlineStr">
         <is>
@@ -8613,24 +8613,24 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D330" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E330" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F330" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="G330" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>2000</v>
+        <v>2013</v>
       </c>
       <c r="B331" t="inlineStr">
         <is>
@@ -8638,24 +8638,24 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D331" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E331" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F331" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="G331" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>2001</v>
+        <v>2014</v>
       </c>
       <c r="B332" t="inlineStr">
         <is>
@@ -8663,24 +8663,24 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D332" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E332" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F332" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="G332" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>2002</v>
+        <v>2015</v>
       </c>
       <c r="B333" t="inlineStr">
         <is>
@@ -8688,24 +8688,24 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D333" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E333" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F333" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="G333" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>2003</v>
+        <v>2016</v>
       </c>
       <c r="B334" t="inlineStr">
         <is>
@@ -8719,7 +8719,7 @@
         <v>4</v>
       </c>
       <c r="E334" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F334" t="n">
         <v>-3</v>
@@ -8730,7 +8730,7 @@
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>2004</v>
+        <v>2017</v>
       </c>
       <c r="B335" t="inlineStr">
         <is>
@@ -8744,7 +8744,7 @@
         <v>4</v>
       </c>
       <c r="E335" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F335" t="n">
         <v>-3</v>
@@ -8755,7 +8755,7 @@
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>2005</v>
+        <v>2018</v>
       </c>
       <c r="B336" t="inlineStr">
         <is>
@@ -8769,7 +8769,7 @@
         <v>4</v>
       </c>
       <c r="E336" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F336" t="n">
         <v>-3</v>
@@ -8780,332 +8780,332 @@
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>2006</v>
+        <v>1991</v>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C337" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D337" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E337" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F337" t="n">
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="G337" t="n">
-        <v>-3</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
-        <v>2007</v>
+        <v>1992</v>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C338" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D338" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E338" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F338" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G338" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>2008</v>
+        <v>1993</v>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C339" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D339" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E339" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F339" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G339" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>2009</v>
+        <v>1994</v>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C340" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D340" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E340" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F340" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G340" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
-        <v>2010</v>
+        <v>1995</v>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C341" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D341" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E341" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F341" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G341" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
-        <v>2011</v>
+        <v>1996</v>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C342" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D342" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E342" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F342" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G342" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>2012</v>
+        <v>1997</v>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C343" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D343" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E343" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F343" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G343" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>2013</v>
+        <v>1998</v>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C344" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D344" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E344" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F344" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G344" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>2014</v>
+        <v>1999</v>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C345" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D345" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E345" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F345" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G345" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="n">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C346" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D346" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E346" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F346" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G346" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C347" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D347" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E347" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F347" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G347" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>2017</v>
+        <v>2002</v>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C348" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D348" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E348" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F348" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G348" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>2018</v>
+        <v>2003</v>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="C349" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D349" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E349" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F349" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="G349" t="n">
-        <v>-3</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>1991</v>
+        <v>2004</v>
       </c>
       <c r="B350" t="inlineStr">
         <is>
@@ -9116,21 +9116,21 @@
         <v>0</v>
       </c>
       <c r="D350" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E350" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F350" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="G350" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
-        <v>1992</v>
+        <v>2005</v>
       </c>
       <c r="B351" t="inlineStr">
         <is>
@@ -9144,7 +9144,7 @@
         <v>9</v>
       </c>
       <c r="E351" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F351" t="n">
         <v>-9</v>
@@ -9155,7 +9155,7 @@
     </row>
     <row r="352">
       <c r="A352" t="n">
-        <v>1993</v>
+        <v>2006</v>
       </c>
       <c r="B352" t="inlineStr">
         <is>
@@ -9169,7 +9169,7 @@
         <v>9</v>
       </c>
       <c r="E352" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F352" t="n">
         <v>-9</v>
@@ -9180,7 +9180,7 @@
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>1994</v>
+        <v>2007</v>
       </c>
       <c r="B353" t="inlineStr">
         <is>
@@ -9194,7 +9194,7 @@
         <v>9</v>
       </c>
       <c r="E353" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F353" t="n">
         <v>-9</v>
@@ -9205,7 +9205,7 @@
     </row>
     <row r="354">
       <c r="A354" t="n">
-        <v>1995</v>
+        <v>2008</v>
       </c>
       <c r="B354" t="inlineStr">
         <is>
@@ -9219,7 +9219,7 @@
         <v>9</v>
       </c>
       <c r="E354" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F354" t="n">
         <v>-9</v>
@@ -9230,7 +9230,7 @@
     </row>
     <row r="355">
       <c r="A355" t="n">
-        <v>1996</v>
+        <v>2009</v>
       </c>
       <c r="B355" t="inlineStr">
         <is>
@@ -9244,7 +9244,7 @@
         <v>9</v>
       </c>
       <c r="E355" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F355" t="n">
         <v>-9</v>
@@ -9255,7 +9255,7 @@
     </row>
     <row r="356">
       <c r="A356" t="n">
-        <v>1997</v>
+        <v>2010</v>
       </c>
       <c r="B356" t="inlineStr">
         <is>
@@ -9269,7 +9269,7 @@
         <v>9</v>
       </c>
       <c r="E356" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F356" t="n">
         <v>-9</v>
@@ -9280,7 +9280,7 @@
     </row>
     <row r="357">
       <c r="A357" t="n">
-        <v>1998</v>
+        <v>2011</v>
       </c>
       <c r="B357" t="inlineStr">
         <is>
@@ -9294,7 +9294,7 @@
         <v>9</v>
       </c>
       <c r="E357" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F357" t="n">
         <v>-9</v>
@@ -9305,7 +9305,7 @@
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>1999</v>
+        <v>2012</v>
       </c>
       <c r="B358" t="inlineStr">
         <is>
@@ -9319,7 +9319,7 @@
         <v>9</v>
       </c>
       <c r="E358" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F358" t="n">
         <v>-9</v>
@@ -9330,7 +9330,7 @@
     </row>
     <row r="359">
       <c r="A359" t="n">
-        <v>2000</v>
+        <v>2013</v>
       </c>
       <c r="B359" t="inlineStr">
         <is>
@@ -9341,21 +9341,21 @@
         <v>0</v>
       </c>
       <c r="D359" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E359" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F359" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="G359" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="n">
-        <v>2001</v>
+        <v>2014</v>
       </c>
       <c r="B360" t="inlineStr">
         <is>
@@ -9366,21 +9366,21 @@
         <v>0</v>
       </c>
       <c r="D360" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E360" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F360" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="G360" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="n">
-        <v>2002</v>
+        <v>2015</v>
       </c>
       <c r="B361" t="inlineStr">
         <is>
@@ -9391,21 +9391,21 @@
         <v>0</v>
       </c>
       <c r="D361" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E361" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F361" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="G361" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="n">
-        <v>2003</v>
+        <v>2016</v>
       </c>
       <c r="B362" t="inlineStr">
         <is>
@@ -9416,21 +9416,21 @@
         <v>0</v>
       </c>
       <c r="D362" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E362" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F362" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="G362" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="n">
-        <v>2004</v>
+        <v>2017</v>
       </c>
       <c r="B363" t="inlineStr">
         <is>
@@ -9441,21 +9441,21 @@
         <v>0</v>
       </c>
       <c r="D363" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E363" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F363" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="G363" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
-        <v>2005</v>
+        <v>2018</v>
       </c>
       <c r="B364" t="inlineStr">
         <is>
@@ -9466,346 +9466,346 @@
         <v>0</v>
       </c>
       <c r="D364" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E364" t="n">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F364" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="G364" t="n">
-        <v>-9</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
-        <v>2006</v>
+        <v>1991</v>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C365" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D365" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E365" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F365" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
       <c r="G365" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
-        <v>2007</v>
+        <v>1992</v>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C366" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D366" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E366" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="F366" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
       <c r="G366" t="n">
-        <v>-9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
-        <v>2008</v>
+        <v>1993</v>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C367" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D367" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E367" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F367" t="n">
-        <v>-9</v>
+        <v>5</v>
       </c>
       <c r="G367" t="n">
-        <v>-9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
-        <v>2009</v>
+        <v>1994</v>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C368" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D368" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E368" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F368" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
       <c r="G368" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="n">
-        <v>2010</v>
+        <v>1995</v>
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C369" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D369" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E369" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F369" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
       <c r="G369" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="n">
-        <v>2011</v>
+        <v>1996</v>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C370" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D370" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E370" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F370" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
       <c r="G370" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
-        <v>2012</v>
+        <v>1997</v>
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C371" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D371" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E371" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F371" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
       <c r="G371" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="n">
-        <v>2013</v>
+        <v>1998</v>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C372" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D372" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E372" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F372" t="n">
-        <v>-8</v>
+        <v>7</v>
       </c>
       <c r="G372" t="n">
-        <v>-8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="n">
-        <v>2014</v>
+        <v>1999</v>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C373" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D373" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E373" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F373" t="n">
-        <v>-8</v>
+        <v>7</v>
       </c>
       <c r="G373" t="n">
-        <v>-8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C374" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D374" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E374" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F374" t="n">
-        <v>-8</v>
+        <v>6</v>
       </c>
       <c r="G374" t="n">
-        <v>-8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C375" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D375" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E375" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F375" t="n">
-        <v>-8</v>
+        <v>6</v>
       </c>
       <c r="G375" t="n">
-        <v>-8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
-        <v>2017</v>
+        <v>2002</v>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C376" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D376" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E376" t="n">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F376" t="n">
-        <v>-8</v>
+        <v>6</v>
       </c>
       <c r="G376" t="n">
-        <v>-8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="n">
-        <v>2018</v>
+        <v>2003</v>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="C377" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D377" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E377" t="n">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F377" t="n">
-        <v>-8</v>
+        <v>6</v>
       </c>
       <c r="G377" t="n">
-        <v>-8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="n">
-        <v>1991</v>
+        <v>2004</v>
       </c>
       <c r="B378" t="inlineStr">
         <is>
@@ -9819,7 +9819,7 @@
         <v>0</v>
       </c>
       <c r="E378" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F378" t="n">
         <v>6</v>
@@ -9830,7 +9830,7 @@
     </row>
     <row r="379">
       <c r="A379" t="n">
-        <v>1992</v>
+        <v>2005</v>
       </c>
       <c r="B379" t="inlineStr">
         <is>
@@ -9844,7 +9844,7 @@
         <v>0</v>
       </c>
       <c r="E379" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F379" t="n">
         <v>6</v>
@@ -9855,7 +9855,7 @@
     </row>
     <row r="380">
       <c r="A380" t="n">
-        <v>1993</v>
+        <v>2006</v>
       </c>
       <c r="B380" t="inlineStr">
         <is>
@@ -9863,24 +9863,24 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D380" t="n">
         <v>0</v>
       </c>
       <c r="E380" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F380" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G380" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
-        <v>1994</v>
+        <v>2007</v>
       </c>
       <c r="B381" t="inlineStr">
         <is>
@@ -9894,7 +9894,7 @@
         <v>0</v>
       </c>
       <c r="E381" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F381" t="n">
         <v>7</v>
@@ -9905,7 +9905,7 @@
     </row>
     <row r="382">
       <c r="A382" t="n">
-        <v>1995</v>
+        <v>2008</v>
       </c>
       <c r="B382" t="inlineStr">
         <is>
@@ -9919,7 +9919,7 @@
         <v>0</v>
       </c>
       <c r="E382" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F382" t="n">
         <v>7</v>
@@ -9930,7 +9930,7 @@
     </row>
     <row r="383">
       <c r="A383" t="n">
-        <v>1996</v>
+        <v>2009</v>
       </c>
       <c r="B383" t="inlineStr">
         <is>
@@ -9944,7 +9944,7 @@
         <v>0</v>
       </c>
       <c r="E383" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F383" t="n">
         <v>7</v>
@@ -9955,7 +9955,7 @@
     </row>
     <row r="384">
       <c r="A384" t="n">
-        <v>1997</v>
+        <v>2010</v>
       </c>
       <c r="B384" t="inlineStr">
         <is>
@@ -9963,24 +9963,24 @@
         </is>
       </c>
       <c r="C384" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D384" t="n">
         <v>0</v>
       </c>
       <c r="E384" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F384" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G384" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="n">
-        <v>1998</v>
+        <v>2011</v>
       </c>
       <c r="B385" t="inlineStr">
         <is>
@@ -9988,24 +9988,24 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D385" t="n">
         <v>0</v>
       </c>
       <c r="E385" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F385" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G385" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="n">
-        <v>1999</v>
+        <v>2012</v>
       </c>
       <c r="B386" t="inlineStr">
         <is>
@@ -10013,24 +10013,24 @@
         </is>
       </c>
       <c r="C386" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D386" t="n">
         <v>0</v>
       </c>
       <c r="E386" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F386" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G386" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
-        <v>2000</v>
+        <v>2013</v>
       </c>
       <c r="B387" t="inlineStr">
         <is>
@@ -10044,7 +10044,7 @@
         <v>0</v>
       </c>
       <c r="E387" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F387" t="n">
         <v>6</v>
@@ -10055,7 +10055,7 @@
     </row>
     <row r="388">
       <c r="A388" t="n">
-        <v>2001</v>
+        <v>2014</v>
       </c>
       <c r="B388" t="inlineStr">
         <is>
@@ -10063,24 +10063,24 @@
         </is>
       </c>
       <c r="C388" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D388" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E388" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F388" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G388" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="n">
-        <v>2002</v>
+        <v>2015</v>
       </c>
       <c r="B389" t="inlineStr">
         <is>
@@ -10088,24 +10088,24 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D389" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E389" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F389" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G389" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>2003</v>
+        <v>2016</v>
       </c>
       <c r="B390" t="inlineStr">
         <is>
@@ -10113,24 +10113,24 @@
         </is>
       </c>
       <c r="C390" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D390" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E390" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F390" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G390" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
-        <v>2004</v>
+        <v>2017</v>
       </c>
       <c r="B391" t="inlineStr">
         <is>
@@ -10138,24 +10138,24 @@
         </is>
       </c>
       <c r="C391" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D391" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E391" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F391" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G391" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
-        <v>2005</v>
+        <v>2018</v>
       </c>
       <c r="B392" t="inlineStr">
         <is>
@@ -10163,349 +10163,349 @@
         </is>
       </c>
       <c r="C392" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D392" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E392" t="n">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F392" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G392" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
-        <v>2006</v>
+        <v>1991</v>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C393" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D393" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E393" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F393" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
       <c r="G393" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="n">
-        <v>2007</v>
+        <v>1992</v>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C394" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D394" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E394" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="F394" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
       <c r="G394" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="n">
-        <v>2008</v>
+        <v>1993</v>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C395" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D395" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E395" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F395" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
       <c r="G395" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="n">
-        <v>2009</v>
+        <v>1994</v>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C396" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D396" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E396" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F396" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
       <c r="G396" t="n">
-        <v>7</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="n">
-        <v>2010</v>
+        <v>1995</v>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C397" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D397" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E397" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F397" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
       <c r="G397" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="n">
-        <v>2011</v>
+        <v>1996</v>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C398" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D398" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E398" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F398" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
       <c r="G398" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="n">
-        <v>2012</v>
+        <v>1997</v>
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C399" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D399" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E399" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F399" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
       <c r="G399" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="n">
-        <v>2013</v>
+        <v>1998</v>
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C400" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D400" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E400" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F400" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
       <c r="G400" t="n">
-        <v>6</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="n">
-        <v>2014</v>
+        <v>1999</v>
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C401" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D401" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E401" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F401" t="n">
-        <v>4</v>
+        <v>-9</v>
       </c>
       <c r="G401" t="n">
-        <v>4</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="n">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C402" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D402" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E402" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F402" t="n">
-        <v>4</v>
+        <v>-9</v>
       </c>
       <c r="G402" t="n">
-        <v>4</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="n">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C403" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D403" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E403" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F403" t="n">
-        <v>4</v>
+        <v>-9</v>
       </c>
       <c r="G403" t="n">
-        <v>4</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="n">
-        <v>2017</v>
+        <v>2002</v>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C404" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D404" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E404" t="n">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F404" t="n">
-        <v>4</v>
+        <v>-9</v>
       </c>
       <c r="G404" t="n">
-        <v>4</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="n">
-        <v>2018</v>
+        <v>2003</v>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="C405" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D405" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E405" t="n">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F405" t="n">
-        <v>4</v>
+        <v>-9</v>
       </c>
       <c r="G405" t="n">
-        <v>4</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="n">
-        <v>1991</v>
+        <v>2004</v>
       </c>
       <c r="B406" t="inlineStr">
         <is>
@@ -10519,7 +10519,7 @@
         <v>9</v>
       </c>
       <c r="E406" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F406" t="n">
         <v>-9</v>
@@ -10530,7 +10530,7 @@
     </row>
     <row r="407">
       <c r="A407" t="n">
-        <v>1992</v>
+        <v>2005</v>
       </c>
       <c r="B407" t="inlineStr">
         <is>
@@ -10544,7 +10544,7 @@
         <v>9</v>
       </c>
       <c r="E407" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F407" t="n">
         <v>-9</v>
@@ -10555,7 +10555,7 @@
     </row>
     <row r="408">
       <c r="A408" t="n">
-        <v>1993</v>
+        <v>2006</v>
       </c>
       <c r="B408" t="inlineStr">
         <is>
@@ -10569,7 +10569,7 @@
         <v>9</v>
       </c>
       <c r="E408" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F408" t="n">
         <v>-9</v>
@@ -10580,7 +10580,7 @@
     </row>
     <row r="409">
       <c r="A409" t="n">
-        <v>1994</v>
+        <v>2007</v>
       </c>
       <c r="B409" t="inlineStr">
         <is>
@@ -10594,7 +10594,7 @@
         <v>9</v>
       </c>
       <c r="E409" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F409" t="n">
         <v>-9</v>
@@ -10605,7 +10605,7 @@
     </row>
     <row r="410">
       <c r="A410" t="n">
-        <v>1995</v>
+        <v>2008</v>
       </c>
       <c r="B410" t="inlineStr">
         <is>
@@ -10619,7 +10619,7 @@
         <v>9</v>
       </c>
       <c r="E410" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F410" t="n">
         <v>-9</v>
@@ -10630,7 +10630,7 @@
     </row>
     <row r="411">
       <c r="A411" t="n">
-        <v>1996</v>
+        <v>2009</v>
       </c>
       <c r="B411" t="inlineStr">
         <is>
@@ -10644,7 +10644,7 @@
         <v>9</v>
       </c>
       <c r="E411" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F411" t="n">
         <v>-9</v>
@@ -10655,7 +10655,7 @@
     </row>
     <row r="412">
       <c r="A412" t="n">
-        <v>1997</v>
+        <v>2010</v>
       </c>
       <c r="B412" t="inlineStr">
         <is>
@@ -10669,7 +10669,7 @@
         <v>9</v>
       </c>
       <c r="E412" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F412" t="n">
         <v>-9</v>
@@ -10680,7 +10680,7 @@
     </row>
     <row r="413">
       <c r="A413" t="n">
-        <v>1998</v>
+        <v>2011</v>
       </c>
       <c r="B413" t="inlineStr">
         <is>
@@ -10694,7 +10694,7 @@
         <v>9</v>
       </c>
       <c r="E413" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F413" t="n">
         <v>-9</v>
@@ -10705,7 +10705,7 @@
     </row>
     <row r="414">
       <c r="A414" t="n">
-        <v>1999</v>
+        <v>2012</v>
       </c>
       <c r="B414" t="inlineStr">
         <is>
@@ -10719,7 +10719,7 @@
         <v>9</v>
       </c>
       <c r="E414" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F414" t="n">
         <v>-9</v>
@@ -10730,7 +10730,7 @@
     </row>
     <row r="415">
       <c r="A415" t="n">
-        <v>2000</v>
+        <v>2013</v>
       </c>
       <c r="B415" t="inlineStr">
         <is>
@@ -10744,7 +10744,7 @@
         <v>9</v>
       </c>
       <c r="E415" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F415" t="n">
         <v>-9</v>
@@ -10755,7 +10755,7 @@
     </row>
     <row r="416">
       <c r="A416" t="n">
-        <v>2001</v>
+        <v>2014</v>
       </c>
       <c r="B416" t="inlineStr">
         <is>
@@ -10769,7 +10769,7 @@
         <v>9</v>
       </c>
       <c r="E416" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F416" t="n">
         <v>-9</v>
@@ -10780,7 +10780,7 @@
     </row>
     <row r="417">
       <c r="A417" t="n">
-        <v>2002</v>
+        <v>2015</v>
       </c>
       <c r="B417" t="inlineStr">
         <is>
@@ -10794,7 +10794,7 @@
         <v>9</v>
       </c>
       <c r="E417" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F417" t="n">
         <v>-9</v>
@@ -10805,7 +10805,7 @@
     </row>
     <row r="418">
       <c r="A418" t="n">
-        <v>2003</v>
+        <v>2016</v>
       </c>
       <c r="B418" t="inlineStr">
         <is>
@@ -10819,7 +10819,7 @@
         <v>9</v>
       </c>
       <c r="E418" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F418" t="n">
         <v>-9</v>
@@ -10830,7 +10830,7 @@
     </row>
     <row r="419">
       <c r="A419" t="n">
-        <v>2004</v>
+        <v>2017</v>
       </c>
       <c r="B419" t="inlineStr">
         <is>
@@ -10844,7 +10844,7 @@
         <v>9</v>
       </c>
       <c r="E419" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F419" t="n">
         <v>-9</v>
@@ -10855,7 +10855,7 @@
     </row>
     <row r="420">
       <c r="A420" t="n">
-        <v>2005</v>
+        <v>2018</v>
       </c>
       <c r="B420" t="inlineStr">
         <is>
@@ -10869,7 +10869,7 @@
         <v>9</v>
       </c>
       <c r="E420" t="n">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F420" t="n">
         <v>-9</v>
@@ -10880,327 +10880,327 @@
     </row>
     <row r="421">
       <c r="A421" t="n">
-        <v>2006</v>
+        <v>1991</v>
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C421" t="n">
         <v>0</v>
       </c>
       <c r="D421" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E421" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F421" t="n">
-        <v>-9</v>
+        <v>-5</v>
       </c>
       <c r="G421" t="n">
-        <v>-9</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="n">
-        <v>2007</v>
+        <v>1992</v>
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C422" t="n">
         <v>0</v>
       </c>
       <c r="D422" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E422" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="F422" t="n">
-        <v>-9</v>
+        <v>-5</v>
       </c>
       <c r="G422" t="n">
-        <v>-9</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="n">
-        <v>2008</v>
+        <v>1993</v>
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C423" t="n">
         <v>0</v>
       </c>
       <c r="D423" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E423" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F423" t="n">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="G423" t="n">
-        <v>-9</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="n">
-        <v>2009</v>
+        <v>1994</v>
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C424" t="n">
         <v>0</v>
       </c>
       <c r="D424" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E424" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F424" t="n">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="G424" t="n">
-        <v>-9</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="n">
-        <v>2010</v>
+        <v>1995</v>
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C425" t="n">
         <v>0</v>
       </c>
       <c r="D425" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E425" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F425" t="n">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="G425" t="n">
-        <v>-9</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="n">
-        <v>2011</v>
+        <v>1996</v>
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C426" t="n">
         <v>0</v>
       </c>
       <c r="D426" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E426" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F426" t="n">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="G426" t="n">
-        <v>-9</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="n">
-        <v>2012</v>
+        <v>1997</v>
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C427" t="n">
         <v>0</v>
       </c>
       <c r="D427" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E427" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F427" t="n">
-        <v>-9</v>
+        <v>-6</v>
       </c>
       <c r="G427" t="n">
-        <v>-9</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="n">
-        <v>2013</v>
+        <v>1998</v>
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C428" t="n">
         <v>0</v>
       </c>
       <c r="D428" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E428" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F428" t="n">
-        <v>-9</v>
+        <v>-6</v>
       </c>
       <c r="G428" t="n">
-        <v>-9</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="n">
-        <v>2014</v>
+        <v>1999</v>
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C429" t="n">
         <v>0</v>
       </c>
       <c r="D429" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E429" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F429" t="n">
-        <v>-9</v>
+        <v>-6</v>
       </c>
       <c r="G429" t="n">
-        <v>-9</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="n">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C430" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D430" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E430" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F430" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
       <c r="G430" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="n">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C431" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D431" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E431" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F431" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
       <c r="G431" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="n">
-        <v>2017</v>
+        <v>2002</v>
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C432" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D432" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E432" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="F432" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
       <c r="G432" t="n">
-        <v>-9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="n">
-        <v>2018</v>
+        <v>1991</v>
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>YGS</t>
         </is>
       </c>
       <c r="C433" t="n">
         <v>0</v>
       </c>
       <c r="D433" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E433" t="n">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F433" t="n">
-        <v>-9</v>
+        <v>-5</v>
       </c>
       <c r="G433" t="n">
-        <v>-9</v>
+        <v>-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>